<commit_message>
Useful Excel Inbuilt Functions
</commit_message>
<xml_diff>
--- a/excel_functions/excel_functions_formulas.xlsx
+++ b/excel_functions/excel_functions_formulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhiraj\Desktop\excel-for-all\excel_inbuilt_functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803E90B-499E-446F-BDFA-DA84E818120A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B2DE38-DE53-435C-A180-A4C2E47ACA8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="10" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Max-Min" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="90">
   <si>
     <t>FirstName</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Hudson</t>
   </si>
   <si>
-    <t>CONCATENATE(B2," ",C2)</t>
-  </si>
-  <si>
     <t>EmployeeID</t>
   </si>
   <si>
@@ -256,18 +253,12 @@
     <t>with NO instances</t>
   </si>
   <si>
-    <t>SUM</t>
-  </si>
-  <si>
     <t>SUMIF</t>
   </si>
   <si>
     <t>SUMIFS</t>
   </si>
   <si>
-    <t>COUNT</t>
-  </si>
-  <si>
     <t>COUNTIF</t>
   </si>
   <si>
@@ -302,6 +293,18 @@
   </si>
   <si>
     <t>Date Right</t>
+  </si>
+  <si>
+    <t>CONCAT(B2," ",C2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SUM (Total Salary)</t>
+  </si>
+  <si>
+    <t>COUNT (salary_counts)</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -687,28 +690,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -725,10 +728,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -762,10 +765,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -791,10 +794,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -820,10 +823,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -849,10 +852,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -878,10 +881,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -898,19 +901,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -936,10 +939,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -965,10 +968,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -993,7 +996,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,12 +1006,12 @@
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1017,25 +1020,25 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1052,10 +1055,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -1065,6 +1068,10 @@
       </c>
       <c r="I2" s="1">
         <v>42253</v>
+      </c>
+      <c r="J2" t="str">
+        <f>_xlfn.CONCAT(B2," ",C2)</f>
+        <v>Jim Halpert</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1081,10 +1088,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -1094,6 +1101,10 @@
       </c>
       <c r="I3" s="1">
         <v>42287</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">_xlfn.CONCAT(B3," ",C3)</f>
+        <v>Pam Beasley</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1110,10 +1121,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -1123,6 +1134,10 @@
       </c>
       <c r="I4" s="1">
         <v>42986</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Dwight Schrute</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1139,10 +1154,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -1152,6 +1167,10 @@
       </c>
       <c r="I5" s="1">
         <v>42341</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Angela Martin</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1168,10 +1187,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -1181,6 +1200,10 @@
       </c>
       <c r="I6" s="1">
         <v>42977</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Toby Flenderson</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1197,10 +1220,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -1210,6 +1233,10 @@
       </c>
       <c r="I7" s="1">
         <v>41528</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael Scott</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1217,19 +1244,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -1239,6 +1266,10 @@
       </c>
       <c r="I8" s="1">
         <v>41551</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Meredith Palmer</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1255,10 +1286,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -1268,6 +1299,10 @@
       </c>
       <c r="I9" s="1">
         <v>42116</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Stanley Hudson</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1284,10 +1319,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -1298,16 +1333,20 @@
       <c r="I10" s="1">
         <v>40800</v>
       </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Kevin Malone</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H11" t="str">
-        <f t="shared" ref="H11:H12" si="0">CONCATENATE(B11," ",C11)</f>
+        <f t="shared" ref="H11:H12" si="1">CONCATENATE(B11," ",C11)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1323,19 +1362,27 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1344,28 +1391,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1382,19 +1429,27 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="J2">
+        <f>_xlfn.DAYS(I2,H2)</f>
+        <v>5056</v>
+      </c>
+      <c r="K2">
+        <f>NETWORKDAYS(H2,I2)</f>
+        <v>3611</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1411,19 +1466,27 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J10" si="0">_xlfn.DAYS(I3,H3)</f>
+        <v>5851</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="1">NETWORKDAYS(H3,I3)</f>
+        <v>4180</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1440,19 +1503,27 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>6275</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>4484</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1469,19 +1540,27 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>5811</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>4152</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1498,19 +1577,27 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>5960</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>4258</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1527,19 +1614,27 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>4511</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>3223</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1547,28 +1642,36 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>3595</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>2568</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1585,19 +1688,27 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>4700</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>3358</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1614,19 +1725,27 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>4273</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>3053</v>
       </c>
     </row>
   </sheetData>
@@ -1654,7 +1773,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1663,28 +1782,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1701,10 +1820,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -1738,10 +1857,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -1775,10 +1894,10 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -1812,10 +1931,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -1849,10 +1968,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -1886,10 +2005,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -1914,19 +2033,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -1960,10 +2079,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -1997,10 +2116,10 @@
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -2043,7 +2162,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2052,28 +2171,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2090,10 +2209,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -2123,10 +2242,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -2156,10 +2275,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -2189,10 +2308,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -2222,10 +2341,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -2255,10 +2374,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -2279,19 +2398,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -2321,10 +2440,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -2354,10 +2473,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -2397,7 +2516,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2406,34 +2525,34 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
       <c r="K1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2450,22 +2569,22 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" t="str">
         <f>LEFT(B2:B10,3)</f>
@@ -2494,22 +2613,22 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K10" si="0">LEFT(B3:B11,3)</f>
@@ -2538,22 +2657,22 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
@@ -2582,22 +2701,22 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
@@ -2626,22 +2745,22 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -2670,22 +2789,22 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -2705,31 +2824,31 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -2758,22 +2877,22 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -2802,22 +2921,22 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -2857,7 +2976,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2866,25 +2985,25 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2901,10 +3020,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -2935,10 +3054,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -2969,10 +3088,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -3003,10 +3122,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -3037,10 +3156,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -3071,10 +3190,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -3096,19 +3215,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -3139,10 +3258,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -3173,10 +3292,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -3211,7 +3330,7 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -3223,7 +3342,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3232,28 +3351,28 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
         <v>67</v>
-      </c>
-      <c r="K1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3270,10 +3389,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -3303,10 +3422,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -3330,16 +3449,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -3369,10 +3488,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -3396,16 +3515,16 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -3429,16 +3548,16 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -3459,19 +3578,19 @@
         <v>1007</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -3495,16 +3614,16 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -3528,16 +3647,16 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10">
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -3566,18 +3685,21 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="K2" sqref="K2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3586,31 +3708,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
-      </c>
-      <c r="L1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3627,19 +3749,31 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="J2" t="str">
+        <f>SUBSTITUTE(H2:H10,"/","-",1)</f>
+        <v>11-2/2001</v>
+      </c>
+      <c r="K2" t="str">
+        <f>SUBSTITUTE(H2:H10,"/","-",2)</f>
+        <v>11/2-2001</v>
+      </c>
+      <c r="L2" t="str">
+        <f>J4</f>
+        <v>7-4/2000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3656,19 +3790,31 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">SUBSTITUTE(H3:H11,"/","-",1)</f>
+        <v>10-3/1999</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K10" si="1">SUBSTITUTE(H3:H11,"/","-",2)</f>
+        <v>10/3-1999</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L10" si="2">SUBSTITUTE(H3:H11,"-","/")</f>
+        <v>10/3/1999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3685,19 +3831,31 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>7-4/2000</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>7/4-2000</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>7/4/2000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3714,19 +3872,31 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>1-5/2000</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>1/5-2000</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>1/5/2000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3743,19 +3913,31 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>5-6/2001</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>5/6-2001</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>5/6/2001</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3772,19 +3954,31 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>5-6/2001</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>5/6-2001</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>5/6/2001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3792,28 +3986,40 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>11-8/2003</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>11/8-2003</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>11/8/2003</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3830,19 +4036,31 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>6-9/2002</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>6/9-2002</v>
+      </c>
+      <c r="L9" t="str">
+        <f>SUBSTITUTE(H9:H17,"-","/")</f>
+        <v>6/9/2002</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3859,19 +4077,31 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>8-10/2003</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>8/10-2003</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>8/10/2003</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3894,19 +4124,22 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
@@ -3924,14 +4157,19 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3940,31 +4178,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
         <v>73</v>
-      </c>
-      <c r="K1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3981,10 +4219,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -3994,6 +4232,18 @@
       </c>
       <c r="I2" s="1">
         <v>42253</v>
+      </c>
+      <c r="J2">
+        <f>SUM(G2:G10)</f>
+        <v>437000</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(G2:G10,"&gt;50000")</f>
+        <v>128000</v>
+      </c>
+      <c r="L2">
+        <f>SUMIFS(G2:G10,E2:E10,"Female",D2:D10,"&gt;30")</f>
+        <v>88000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4010,10 +4260,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -4039,10 +4289,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -4068,10 +4318,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -4097,10 +4347,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -4126,10 +4376,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -4146,19 +4396,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -4184,10 +4434,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -4213,10 +4463,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>
@@ -4240,19 +4490,22 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="41.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4261,31 +4514,31 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
       <c r="J1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4302,10 +4555,10 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>45000</v>
@@ -4315,6 +4568,18 @@
       </c>
       <c r="I2" s="1">
         <v>42253</v>
+      </c>
+      <c r="J2">
+        <f>COUNT(G2:G10)</f>
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(G2:G10,"&gt;45000")</f>
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIFS(A2:A10,"&gt;1005",E2:E10,"Male")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4331,10 +4596,10 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -4360,10 +4625,10 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>63000</v>
@@ -4389,10 +4654,10 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>47000</v>
@@ -4418,10 +4683,10 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>50000</v>
@@ -4447,10 +4712,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7">
         <v>65000</v>
@@ -4467,19 +4732,19 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>41000</v>
@@ -4505,10 +4770,10 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>48000</v>
@@ -4534,10 +4799,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>42000</v>

</xml_diff>